<commit_message>
result on holdout dataset
</commit_message>
<xml_diff>
--- a/training_features/2024-12-14_11-13-51/scores_llama3.1_8b_0-shot_500.xlsx
+++ b/training_features/2024-12-14_11-13-51/scores_llama3.1_8b_0-shot_500.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,50 +456,15 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>xgboost-mse</t>
+          <t>xgboost-y_drop</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>xgboost-mae</t>
+          <t>lasso-y_drop</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>xgboost-rmse</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>xgboost-r2</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>xgboost-k-fold-mse</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>xgboost-k-fold-mae</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>xgboost-k-fold-rmse</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>xgboost-k-fold-r2</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>lasso-y_drop</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>num_datasets</t>
         </is>
@@ -519,80 +484,63 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[[-0.12302472]
+          <t>[[-0.02142273]
+ [ 0.03085009]
+ [-0.01658338]
+ [-0.08774961]
+ [ 0.07629745]
  [ 0.01285947]
+ [-0.1510179 ]
+ [ 0.12167721]
+ [ 0.02495436]
+ [-0.12302472]
+ [-0.00984156]
+ [ 0.14192943]
  [ 0.17040717]
+ [-0.0973577 ]
  [ 0.09454775]
- [-0.00984156]
- [ 0.02495436]
- [-0.02142273]
- [ 0.03085009]
- [-0.0120889 ]
+ [-0.13742305]
  [-0.10978463]
- [-0.08774961]
- [-0.01658338]
- [ 0.14192943]
- [-0.1510179 ]
- [ 0.07629745]
- [-0.13742305]
- [-0.0973577 ]
- [ 0.12167721]]</t>
+ [-0.0120889 ]]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[[-0.05056708]
+          <t>[[-0.13329466]
+ [-0.0755709 ]
+ [ 0.07038691]
+ [-0.00164962]
+ [ 0.03918755]
  [-0.02697289]
+ [-0.1761752 ]
+ [ 0.2074219 ]
+ [-0.00913573]
+ [-0.05056708]
+ [-0.11520114]
+ [ 0.21395498]
  [ 0.23900712]
+ [-0.01852215]
  [ 0.17288869]
- [-0.11520114]
- [-0.00913573]
- [-0.13329466]
- [-0.0755709 ]
- [-0.12252524]
+ [-0.17013782]
  [-0.13586598]
- [-0.00164962]
- [ 0.07038691]
- [ 0.21395498]
- [-0.1761752 ]
- [ 0.03918755]
- [-0.17013782]
- [-0.01852215]
- [ 0.2074219 ]]</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
+ [-0.12252524]]</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>[-0.01534459  0.2239905   0.02075964  0.03055483  0.2244603  -0.00801081
+ -0.0942831   0.0306251  -0.00213945 -0.00791237 -0.00733042  0.06793422
+ -0.00980453 -0.00111156 -0.0084103  -0.18789811 -0.02736913  0.0831384 ]</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>[-0.02183669  0.02984185 -0.00529348 -0.0746076   0.06522541  0.00451568
+ -0.14802472  0.11230291  0.01416389 -0.10475166 -0.0128725   0.12858878
+  0.15872908 -0.08089117  0.08777961 -0.13037342 -0.10517074 -0.01009647]</t>
+        </is>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>[-0.11219881  0.00747428  0.16375266  0.08999354 -0.01192643  0.01810761
- -0.0218786   0.02999941 -0.01124746 -0.10566076 -0.08017642 -0.00993135
-  0.13423354 -0.14843054  0.06918397 -0.13178362 -0.08772221  0.11543996]</t>
-        </is>
-      </c>
-      <c r="O2" t="n">
         <v>14</v>
       </c>
     </row>
@@ -610,80 +558,65 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[[-0.15734918]
- [-0.03055012]
- [ 0.01042418]
- [-0.04834132]
- [-0.02010913]
+          <t>[[ 0.07821837]
+ [-0.15734918]
  [ 0.02657613]
+ [-0.00395006]
+ [-0.03550372]
  [ 0.04690658]
- [-0.03550372]
- [-0.00395006]
- [ 0.08316006]
- [-0.01515553]
- [-0.14350568]
- [ 0.06437487]
  [ 0.04993961]
  [ 0.15074391]
- [ 0.07821837]
+ [ 0.01042418]
+ [ 0.08316006]
+ [-0.03055012]
+ [-0.02010913]
+ [ 0.06437487]
  [-0.17307925]
- [ 0.02442902]]</t>
+ [ 0.02442902]
+ [-0.14350568]
+ [-0.01515553]
+ [-0.04834132]]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[[-0.16755368]
- [-0.04599812]
- [ 0.00536362]
- [-0.05645174]
- [-0.0038856 ]
+          <t>[[ 0.11549848]
+ [-0.16755368]
  [ 0.01758147]
+ [-0.01034481]
+ [-0.03462524]
  [ 0.05721805]
- [-0.03462524]
- [-0.01034481]
- [ 0.07311682]
- [-0.01525848]
- [-0.15903066]
- [ 0.10697546]
  [ 0.04972808]
  [ 0.14122358]
- [ 0.11549848]
+ [ 0.00536362]
+ [ 0.07311682]
+ [-0.04599812]
+ [-0.0038856 ]
+ [ 0.10697546]
  [-0.18829422]
- [ 0.02196575]]</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
+ [ 0.02196575]
+ [-0.15903066]
+ [-0.01525848]
+ [-0.05645174]]</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>[ 0.0755531  -0.07964763 -0.03116396  0.01566319 -0.0019985   0.14138444
+  0.07730947  0.08924988 -0.0171617   0.07567372 -0.03096188 -0.0019985
+  0.05287367 -0.04099603  0.13360655 -0.12689601 -0.03096188  0.01770351]</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>[ 9.27115254e-02 -1.65547540e-01  1.62093408e-02 -1.53449298e-02
+ -3.52491453e-02  5.71114641e-02  5.04963199e-02  1.56787913e-01
+ -5.70181680e-05  8.77986307e-02 -3.00183872e-02 -1.09736062e-02
+  7.87387679e-02 -1.82008811e-01  2.45032651e-02 -1.51574783e-01
+ -5.74284815e-03 -6.06114024e-02]</t>
+        </is>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>[-0.16376414 -0.03411636 -0.00403394 -0.06693836 -0.00169622  0.00908983
-  0.06107367 -0.02644702 -0.02091381  0.0745438  -0.00936556 -0.15402317
-  0.0936135   0.05745892  0.14301228  0.10335446 -0.18364992  0.03003081]</t>
-        </is>
-      </c>
-      <c r="O3" t="n">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
holdout set set results
</commit_message>
<xml_diff>
--- a/training_features/2024-12-14_11-13-51/scores_llama3.1_8b_0-shot_500.xlsx
+++ b/training_features/2024-12-14_11-13-51/scores_llama3.1_8b_0-shot_500.xlsx
@@ -484,60 +484,50 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[[-0.02142273]
- [ 0.03085009]
- [-0.01658338]
- [-0.08774961]
- [ 0.07629745]
- [ 0.01285947]
- [-0.1510179 ]
- [ 0.12167721]
- [ 0.02495436]
- [-0.12302472]
- [-0.00984156]
- [ 0.14192943]
- [ 0.17040717]
- [-0.0973577 ]
- [ 0.09454775]
- [-0.13742305]
- [-0.10978463]
- [-0.0120889 ]]</t>
+          <t>[[-0.01259479]
+ [ 0.03034212]
+ [ 0.06248812]
+ [ 0.02095435]
+ [-0.05816003]
+ [-0.1876165 ]
+ [-0.0685947 ]
+ [ 0.03341826]
+ [ 0.14568317]
+ [ 0.0732327 ]
+ [ 0.0585992 ]
+ [ 0.08114034]
+ [-0.22276638]]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[[-0.13329466]
- [-0.0755709 ]
- [ 0.07038691]
- [-0.00164962]
- [ 0.03918755]
- [-0.02697289]
- [-0.1761752 ]
- [ 0.2074219 ]
- [-0.00913573]
- [-0.05056708]
- [-0.11520114]
- [ 0.21395498]
- [ 0.23900712]
- [-0.01852215]
- [ 0.17288869]
- [-0.17013782]
- [-0.13586598]
- [-0.12252524]]</t>
+          <t>[[-0.00512007]
+ [-0.02061025]
+ [ 0.15090641]
+ [ 0.01116715]
+ [ 0.07244902]
+ [-0.16741335]
+ [ 0.10327631]
+ [ 0.05800829]
+ [ 0.08898542]
+ [ 0.05498782]
+ [-0.05554802]
+ [-0.07891823]
+ [-0.25604462]]</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[-0.01534459  0.2239905   0.02075964  0.03055483  0.2244603  -0.00801081
- -0.0942831   0.0306251  -0.00213945 -0.00791237 -0.00733042  0.06793422
- -0.00980453 -0.00111156 -0.0084103  -0.18789811 -0.02736913  0.0831384 ]</t>
+          <t>[-0.00728113  0.03071338 -0.07319244 -0.01381209 -0.13809748 -0.02902286
+ -0.09674671  0.01028812  0.03443562  0.04515991  0.09864035 -0.16041014
+ -0.02462132]</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[-0.02183669  0.02984185 -0.00529348 -0.0746076   0.06522541  0.00451568
- -0.14802472  0.11230291  0.01416389 -0.10475166 -0.0128725   0.12858878
-  0.15872908 -0.08089117  0.08777961 -0.13037342 -0.10517074 -0.01009647]</t>
+          <t>[-0.00929498  0.03179126  0.05999124  0.02234818 -0.05756453 -0.18848256
+ -0.07088835  0.03299387  0.14752245  0.0740176   0.06037279  0.08233421
+ -0.22901532]</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -558,62 +548,50 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[[ 0.07821837]
- [-0.15734918]
- [ 0.02657613]
- [-0.00395006]
- [-0.03550372]
- [ 0.04690658]
- [ 0.04993961]
- [ 0.15074391]
- [ 0.01042418]
- [ 0.08316006]
- [-0.03055012]
- [-0.02010913]
- [ 0.06437487]
- [-0.17307925]
- [ 0.02442902]
- [-0.14350568]
- [-0.01515553]
- [-0.04834132]]</t>
+          <t>[[ 0.1021785 ]
+ [-0.01395554]
+ [-0.04214394]
+ [-0.10800695]
+ [ 0.10941466]
+ [ 0.01154953]
+ [ 0.06453123]
+ [-0.01845728]
+ [-0.03349375]
+ [ 0.00092294]
+ [-0.01551101]
+ [-0.10548255]
+ [ 0.00458001]]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[[ 0.11549848]
- [-0.16755368]
- [ 0.01758147]
- [-0.01034481]
- [-0.03462524]
- [ 0.05721805]
- [ 0.04972808]
- [ 0.14122358]
- [ 0.00536362]
- [ 0.07311682]
- [-0.04599812]
- [-0.0038856 ]
- [ 0.10697546]
- [-0.18829422]
- [ 0.02196575]
- [-0.15903066]
- [-0.01525848]
- [-0.05645174]]</t>
+          <t>[[ 0.06842089]
+ [-0.0793725 ]
+ [-0.05879938]
+ [-0.077634  ]
+ [ 0.08275873]
+ [-0.03398016]
+ [ 0.08914596]
+ [-0.04155097]
+ [ 0.0043805 ]
+ [ 0.0708936 ]
+ [-0.00629081]
+ [-0.07195538]
+ [ 0.01010939]]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[ 0.0755531  -0.07964763 -0.03116396  0.01566319 -0.0019985   0.14138444
-  0.07730947  0.08924988 -0.0171617   0.07567372 -0.03096188 -0.0019985
-  0.05287367 -0.04099603  0.13360655 -0.12689601 -0.03096188  0.01770351]</t>
+          <t>[ 0.05118617 -0.08705603 -0.01671972 -0.05980253  0.02321769  0.03433534
+  0.01032242  0.0184057  -0.12173654 -0.05782419  0.00099413 -0.14246176
+ -0.01087969]</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>[ 9.27115254e-02 -1.65547540e-01  1.62093408e-02 -1.53449298e-02
- -3.52491453e-02  5.71114641e-02  5.04963199e-02  1.56787913e-01
- -5.70181680e-05  8.77986307e-02 -3.00183872e-02 -1.09736062e-02
-  7.87387679e-02 -1.82008811e-01  2.45032651e-02 -1.51574783e-01
- -5.74284815e-03 -6.06114024e-02]</t>
+          <t>[ 0.09550865 -0.01066191 -0.03435089 -0.10577454  0.10775223  0.00708206
+  0.06304329 -0.01701662 -0.03901747  0.00908708 -0.01760989 -0.1065105
+  0.00459438]</t>
         </is>
       </c>
       <c r="H3" t="n">

</xml_diff>